<commit_message>
docs: azure services cost updated. this fixed #5
</commit_message>
<xml_diff>
--- a/pricing/EstimatedCost.xlsx
+++ b/pricing/EstimatedCost.xlsx
@@ -59,13 +59,13 @@
     <t>Azure Databricks</t>
   </si>
   <si>
-    <t>Charge de travail Jobs Compute avec Photon, Niveau Premium, 1 F4S (4 vCPU(s), 8 GO DE RAM) x 40 Heures, À l'utilisation, 1.25 DBU x 40 Heures</t>
+    <t>Charge de travail Calcul à usage général, Niveau Premium, 1 F4S (4 vCPU(s), 8 GO DE RAM) x 40 Heures, À l'utilisation, 0.5 DBU x 40 Heures</t>
   </si>
   <si>
     <t>Power BI Embedded</t>
   </si>
   <si>
-    <t>1 nœuds x 40 Heures, type de nœud : A1, 1 cœurs virtuels, 3 Go de RAM, 1-300 rendus maximum/heure</t>
+    <t>1 nœuds x 5 Heures, type de nœud : A1, 1 cœurs virtuels, 3 Go de RAM, 1-300 rendus maximum/heure</t>
   </si>
   <si>
     <t>Support</t>
@@ -92,7 +92,7 @@
     <t>All prices shown are in United States – Dollar ($) USD. This is a summary estimate, not a quote. For up to date pricing information please visit https://azure.microsoft.com/pricing/calculator/</t>
   </si>
   <si>
-    <t>This estimate was created at 12/18/2023 1:47:57 PM UTC.</t>
+    <t>This estimate was created at 12/19/2023 8:24:19 AM UTC.</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="5">
-        <v>23.08</v>
+        <v>19.08</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -449,7 +449,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="5">
-        <v>40.324</v>
+        <v>5.0405</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -615,7 +615,7 @@
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="15">
-        <v>64.032</v>
+        <v>24.7485</v>
       </c>
       <c r="G11" s="15">
         <v>0</v>

</xml_diff>